<commit_message>
added few more DB validation in my test suite
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TaskCreation.xlsx
+++ b/src/test/resources/testData/TaskCreation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19163\seleniumArchitecture\QDPM\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E028726B-D718-47F8-8B9F-DE68DA2AAF82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39B0A64-94D0-4ADA-98D0-4854F95330BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>